<commit_message>
MV and MEMLDA assembly commands added
</commit_message>
<xml_diff>
--- a/Documentation/ALU Codes.xlsx
+++ b/Documentation/ALU Codes.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9336" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9336" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="ALU Codes" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="88">
   <si>
     <t>ALU CODE</t>
   </si>
@@ -251,6 +251,45 @@
   </si>
   <si>
     <t>Halt the processor</t>
+  </si>
+  <si>
+    <t>move content from A to B</t>
+  </si>
+  <si>
+    <t>0x31</t>
+  </si>
+  <si>
+    <t>GP1</t>
+  </si>
+  <si>
+    <t>010</t>
+  </si>
+  <si>
+    <t>000010</t>
+  </si>
+  <si>
+    <t>mv</t>
+  </si>
+  <si>
+    <t>mv &lt;op1&gt; &lt;op2&gt;</t>
+  </si>
+  <si>
+    <t>op1 = source register (in 4 bit value), op2 = destination register (in 4 bit value)</t>
+  </si>
+  <si>
+    <t>memlda</t>
+  </si>
+  <si>
+    <t>0x35</t>
+  </si>
+  <si>
+    <t>load from memory to A</t>
+  </si>
+  <si>
+    <t>memlda &lt;op1&gt;</t>
+  </si>
+  <si>
+    <t>FTREG</t>
   </si>
 </sst>
 </file>
@@ -606,7 +645,7 @@
   <dimension ref="B4:I23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="A13" sqref="A13:XFD13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1044,14 +1083,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:G27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="8.88671875" style="1"/>
-    <col min="4" max="4" width="19.21875" customWidth="1"/>
+    <col min="4" max="4" width="25.5546875" customWidth="1"/>
     <col min="6" max="6" width="14.44140625" style="3" customWidth="1"/>
     <col min="7" max="7" width="34.6640625" customWidth="1"/>
   </cols>
@@ -1170,7 +1209,38 @@
         <v>70</v>
       </c>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B18" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C18" t="s">
+        <v>80</v>
+      </c>
+      <c r="D18" t="s">
+        <v>75</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="G18" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B20" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C20" t="s">
+        <v>83</v>
+      </c>
+      <c r="D20" t="s">
+        <v>85</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B27" s="1" t="s">
         <v>72</v>
       </c>
@@ -1191,8 +1261,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J31" sqref="J31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1312,17 +1382,31 @@
       <c r="F8" s="3"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
+      <c r="A9" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>79</v>
+      </c>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
+      <c r="A10" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>59</v>
+      </c>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>

</xml_diff>